<commit_message>
Updating results documentation with MLP and Naive Bayes results
</commit_message>
<xml_diff>
--- a/documentation/Results.xlsx
+++ b/documentation/Results.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davigrossihasuda/Documents/ITA/TG/tg-differential-privacy/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8226A0E7-15A1-B54C-B632-83D92634794A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82738501-CEC2-474B-80CC-A620B2E64BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20400" yWindow="1220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{788FEABF-C896-4644-B5AB-9B7AB986D1F6}"/>
+    <workbookView xWindow="20400" yWindow="1220" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{788FEABF-C896-4644-B5AB-9B7AB986D1F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Decision Tree" sheetId="1" r:id="rId1"/>
     <sheet name="SVM" sheetId="2" r:id="rId2"/>
+    <sheet name="Naïve Bayes" sheetId="3" r:id="rId3"/>
+    <sheet name="MLP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>Dataset</t>
   </si>
@@ -70,6 +72,12 @@
   </si>
   <si>
     <t>Accuracy (%)</t>
+  </si>
+  <si>
+    <t>breastCancerDataProvider</t>
+  </si>
+  <si>
+    <t>breastCancerAdapter</t>
   </si>
 </sst>
 </file>
@@ -170,9 +178,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -507,110 +516,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>80000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>0.3</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>71.236460436937705</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>0.03</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>67.314003120983998</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>0.03</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>40.279052689553801</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>0.3</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>60.9693409216082</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>0.3</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>29.875390123003399</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -621,6 +630,251 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569A7802-53C0-914D-85C2-DFDBB62A616E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>94.736842105263094</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="7">
+        <v>93.567251461988207</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>87.719298245613999</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>87.719298245613999</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8">
+        <v>59.649122807017498</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0EE78-51DB-DE4F-8A39-8016F79640FE}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="A1:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5">
+        <v>80000</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <v>92.397660818713405</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>89.473684210526301</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>84.210526315789394</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8">
+        <v>86.549707602339097</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8">
+        <v>71.345029239766006</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="34" spans="4:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="D34" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC629143-33C2-944E-9CDD-CCD67B7B5DCB}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
@@ -628,110 +882,110 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5">
         <v>80000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>0.3</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
-        <v>94.736842105263094</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" s="8">
+        <v>40.350877192982402</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C6" s="6">
-        <v>93.567251461988207</v>
-      </c>
-      <c r="D6" s="4"/>
+      <c r="B6" s="5">
+        <v>100</v>
+      </c>
+      <c r="C6" s="8">
+        <v>59.649122807017498</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="7">
-        <v>87.719298245613999</v>
-      </c>
-      <c r="D7" s="4"/>
+      <c r="B7" s="5">
+        <v>100</v>
+      </c>
+      <c r="C7" s="8">
+        <v>59.649122807017498</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2">
-        <v>87.719298245613999</v>
-      </c>
-      <c r="D8" s="4"/>
+      <c r="B8" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="8">
+        <v>59.649122807017498</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="5">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="8">
         <v>59.649122807017498</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing some problems in decision tree notebook
</commit_message>
<xml_diff>
--- a/documentation/Results.xlsx
+++ b/documentation/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davigrossihasuda/Documents/ITA/TG/tg-differential-privacy/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82738501-CEC2-474B-80CC-A620B2E64BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458DEA5B-AD55-984B-888F-992BAC5AF475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20400" yWindow="1220" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{788FEABF-C896-4644-B5AB-9B7AB986D1F6}"/>
+    <workbookView xWindow="10540" yWindow="840" windowWidth="20520" windowHeight="17480" activeTab="1" xr2:uid="{788FEABF-C896-4644-B5AB-9B7AB986D1F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Decision Tree" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="143" workbookViewId="0">
-      <selection sqref="A1:D9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{569A7802-53C0-914D-85C2-DFDBB62A616E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0EE78-51DB-DE4F-8A39-8016F79640FE}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="A1:D9"/>
+    <sheetView zoomScale="210" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -875,11 +875,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC629143-33C2-944E-9CDD-CCD67B7B5DCB}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="209" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">

</xml_diff>